<commit_message>
Started working on RestAssured framework to get data from openweathermap
</commit_message>
<xml_diff>
--- a/src/main/resources/test/data/dataExcel.xlsx
+++ b/src/main/resources/test/data/dataExcel.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cp\eclipse-workspace\WeatherReport0001\src\main\resources\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B0BD740-87F6-408B-B51A-1F963A4CD092}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C46A7776-90BC-424F-A78D-985D7E6841B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{BBC9B369-1E26-4ED4-AF77-86BE22BE0936}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="listOfCities" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -401,9 +401,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A00056-2EFE-4C71-9B7A-30136FB9011D}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Rest Assured framework merged and data is being written to xls properly
</commit_message>
<xml_diff>
--- a/src/main/resources/test/data/dataExcel.xlsx
+++ b/src/main/resources/test/data/dataExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cp\eclipse-workspace\WeatherReport0001\src\main\resources\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACF11945-7913-4CB3-854E-D9786735B40F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{076F7DCD-EB51-4C3E-8D77-E2BC06B404F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{BBC9B369-1E26-4ED4-AF77-86BE22BE0936}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="34">
   <si>
     <t>City</t>
   </si>
@@ -57,19 +57,31 @@
     <t>Humidity (NDTV)</t>
   </si>
   <si>
-    <t>30.0</t>
-  </si>
-  <si>
-    <t>30.00</t>
-  </si>
-  <si>
-    <t>27.0</t>
-  </si>
-  <si>
-    <t>31.3799991607666</t>
-  </si>
-  <si>
-    <t>84</t>
+    <t>Humidity Compare Result</t>
+  </si>
+  <si>
+    <t>LiveTemp Compare Result</t>
+  </si>
+  <si>
+    <t>Max Temp Compare Result</t>
+  </si>
+  <si>
+    <t>Wind Compare Result</t>
+  </si>
+  <si>
+    <t>Wind (OpenWeatherMap)</t>
+  </si>
+  <si>
+    <t>Wind (NDTV)</t>
+  </si>
+  <si>
+    <t>29.00</t>
+  </si>
+  <si>
+    <t>89</t>
+  </si>
+  <si>
+    <t>1.00</t>
   </si>
   <si>
     <t>27.00</t>
@@ -78,10 +90,43 @@
     <t>88</t>
   </si>
   <si>
-    <t>31.38</t>
-  </si>
-  <si>
-    <t>58</t>
+    <t>2.60</t>
+  </si>
+  <si>
+    <t>30.38</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>5.60</t>
+  </si>
+  <si>
+    <t>Weather Condition (OpenWeatherMap)</t>
+  </si>
+  <si>
+    <t>Weather Condition (NDTV)</t>
+  </si>
+  <si>
+    <t>Weather Condition Compare Result</t>
+  </si>
+  <si>
+    <t>Mist&amp;mist</t>
+  </si>
+  <si>
+    <t>Clouds&amp;few clouds</t>
+  </si>
+  <si>
+    <t>Clouds&amp;overcast clouds</t>
+  </si>
+  <si>
+    <t>Mist &amp; mist</t>
+  </si>
+  <si>
+    <t>Clouds &amp; few clouds</t>
+  </si>
+  <si>
+    <t>Clouds &amp; overcast clouds</t>
   </si>
 </sst>
 </file>
@@ -127,10 +172,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -446,28 +498,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A00056-2EFE-4C71-9B7A-30136FB9011D}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="28.28125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="22.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="29.1484375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="29.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="27.86328125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="28.0" collapsed="true"/>
-    <col min="8" max="8" style="1" width="9.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="23.7109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="20.140625" collapsed="true"/>
-    <col min="11" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="16.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="18.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="29.1484375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="17.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="24.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="36.74609375" collapsed="true"/>
+    <col min="9" max="10" customWidth="true" style="1" width="24.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="27.86328125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="1" width="16.42578125" collapsed="true"/>
+    <col min="13" max="13" style="1" width="9.140625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="24.45703125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="20.140625" collapsed="true"/>
+    <col min="16" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -478,46 +534,108 @@
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" t="s">
+      <c r="N2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
       <c r="C3" s="2"/>
-      <c r="I3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
       <c r="C4" s="2"/>
-      <c r="I4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
backend and frontend Framework completed, excel fetch and write working, variance logic for temp implemented, more data comparision left
</commit_message>
<xml_diff>
--- a/src/main/resources/test/data/dataExcel.xlsx
+++ b/src/main/resources/test/data/dataExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cp\eclipse-workspace\WeatherReport0001\src\main\resources\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{076F7DCD-EB51-4C3E-8D77-E2BC06B404F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC73BF1-D794-426A-B85A-556264E325E9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{BBC9B369-1E26-4ED4-AF77-86BE22BE0936}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="60">
   <si>
     <t>City</t>
   </si>
@@ -42,18 +42,12 @@
     <t>LiveTemp (OpenWeatherMap)</t>
   </si>
   <si>
-    <t>Max Temp (OpenWeatherMap)</t>
-  </si>
-  <si>
     <t>Humidity (OpenWeatherMap)</t>
   </si>
   <si>
     <t>LiveTemp (NDTV)</t>
   </si>
   <si>
-    <t>Max Temp (NDTV)</t>
-  </si>
-  <si>
     <t>Humidity (NDTV)</t>
   </si>
   <si>
@@ -63,9 +57,6 @@
     <t>LiveTemp Compare Result</t>
   </si>
   <si>
-    <t>Max Temp Compare Result</t>
-  </si>
-  <si>
     <t>Wind Compare Result</t>
   </si>
   <si>
@@ -75,58 +66,148 @@
     <t>Wind (NDTV)</t>
   </si>
   <si>
+    <t>Weather Condition (OpenWeatherMap)</t>
+  </si>
+  <si>
+    <t>Weather Condition (NDTV)</t>
+  </si>
+  <si>
+    <t>Weather Condition Compare Result</t>
+  </si>
+  <si>
+    <t>Coimbatore</t>
+  </si>
+  <si>
+    <t>Kolkata</t>
+  </si>
+  <si>
+    <t>Mumbai</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>2.35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Humid and Overcast
+</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>2.68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Humid and Mostly Cloudy
+</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>2.8499999999999996</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>4.5600000000000005</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>97</t>
+  </si>
+  <si>
+    <t>8.375</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rain and Humid
+</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>7.15</t>
+  </si>
+  <si>
     <t>29.00</t>
   </si>
   <si>
     <t>89</t>
   </si>
   <si>
-    <t>1.00</t>
-  </si>
-  <si>
-    <t>27.00</t>
-  </si>
-  <si>
-    <t>88</t>
+    <t>Mist and mist</t>
+  </si>
+  <si>
+    <t>Rain and light rain</t>
+  </si>
+  <si>
+    <t>23.00</t>
+  </si>
+  <si>
+    <t>94</t>
   </si>
   <si>
     <t>2.60</t>
   </si>
   <si>
-    <t>30.38</t>
-  </si>
-  <si>
-    <t>59</t>
-  </si>
-  <si>
-    <t>5.60</t>
-  </si>
-  <si>
-    <t>Weather Condition (OpenWeatherMap)</t>
-  </si>
-  <si>
-    <t>Weather Condition (NDTV)</t>
-  </si>
-  <si>
-    <t>Weather Condition Compare Result</t>
-  </si>
-  <si>
-    <t>Mist&amp;mist</t>
-  </si>
-  <si>
-    <t>Clouds&amp;few clouds</t>
-  </si>
-  <si>
-    <t>Clouds&amp;overcast clouds</t>
-  </si>
-  <si>
-    <t>Mist &amp; mist</t>
-  </si>
-  <si>
-    <t>Clouds &amp; few clouds</t>
-  </si>
-  <si>
-    <t>Clouds &amp; overcast clouds</t>
+    <t>28.00</t>
+  </si>
+  <si>
+    <t>30.00</t>
+  </si>
+  <si>
+    <t>4.60</t>
+  </si>
+  <si>
+    <t>Haze and haze</t>
+  </si>
+  <si>
+    <t>1.78</t>
+  </si>
+  <si>
+    <t>26.00</t>
+  </si>
+  <si>
+    <t>3.10</t>
+  </si>
+  <si>
+    <t>28.97</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>5.47</t>
+  </si>
+  <si>
+    <t>Clouds and few clouds</t>
+  </si>
+  <si>
+    <t>4.97</t>
+  </si>
+  <si>
+    <t>Temperatues are NOT within Variance Range</t>
+  </si>
+  <si>
+    <t>Temperatues are within Variance Range</t>
   </si>
 </sst>
 </file>
@@ -498,32 +579,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A00056-2EFE-4C71-9B7A-30136FB9011D}">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D2:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="28.28125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="16.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="18.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="29.1484375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="17.140625" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" style="1" width="17.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="28.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="16.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="41.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="36.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="25.0" collapsed="true"/>
     <col min="7" max="7" customWidth="true" style="1" width="24.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="36.74609375" collapsed="true"/>
-    <col min="9" max="10" customWidth="true" style="1" width="24.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="27.86328125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="1" width="16.42578125" collapsed="true"/>
-    <col min="13" max="13" style="1" width="9.140625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="24.45703125" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="20.140625" collapsed="true"/>
-    <col min="16" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="27.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="16.140625" collapsed="true"/>
+    <col min="10" max="10" style="1" width="9.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="24.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="20.5703125" collapsed="true"/>
+    <col min="13" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -531,110 +610,229 @@
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>59</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>41</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
       </c>
       <c r="H2" t="s">
-        <v>31</v>
-      </c>
-      <c r="K2" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>18</v>
+        <v>40</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L2" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+        <v>51</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>49</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
       </c>
       <c r="H3" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3" t="s">
-        <v>20</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>21</v>
+        <v>44</v>
+      </c>
+      <c r="I3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="L3" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="L4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="H5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" t="s">
+        <v>45</v>
+      </c>
+      <c r="L5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s">
         <v>33</v>
       </c>
-      <c r="K4" t="s">
-        <v>23</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>24</v>
+      <c r="D6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" t="s">
+        <v>57</v>
+      </c>
+      <c r="L6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" t="s">
+        <v>37</v>
+      </c>
+      <c r="K7" t="s">
+        <v>48</v>
+      </c>
+      <c r="L7" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Compare login almost complete for 4 Weather Data points
</commit_message>
<xml_diff>
--- a/src/main/resources/test/data/dataExcel.xlsx
+++ b/src/main/resources/test/data/dataExcel.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cp\eclipse-workspace\WeatherReport0001\src\main\resources\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC73BF1-D794-426A-B85A-556264E325E9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD24AE1-4872-492C-9E09-C86FE4010277}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{BBC9B369-1E26-4ED4-AF77-86BE22BE0936}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="60">
   <si>
     <t>City</t>
   </si>
@@ -82,139 +82,139 @@
   </si>
   <si>
     <t>Mumbai</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>62</t>
-  </si>
-  <si>
-    <t>2.35</t>
   </si>
   <si>
     <t xml:space="preserve">Humid and Overcast
 </t>
   </si>
   <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>63</t>
-  </si>
-  <si>
-    <t>2.68</t>
-  </si>
-  <si>
     <t xml:space="preserve">Humid and Mostly Cloudy
 </t>
   </si>
   <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>2.8499999999999996</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>65</t>
-  </si>
-  <si>
-    <t>4.5600000000000005</t>
-  </si>
-  <si>
     <t>29</t>
   </si>
   <si>
-    <t>97</t>
-  </si>
-  <si>
-    <t>8.375</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rain and Humid
+    <t>29.00</t>
+  </si>
+  <si>
+    <t>89</t>
+  </si>
+  <si>
+    <t>Mist and mist</t>
+  </si>
+  <si>
+    <t>Rain and light rain</t>
+  </si>
+  <si>
+    <t>94</t>
+  </si>
+  <si>
+    <t>Haze and haze</t>
+  </si>
+  <si>
+    <t>Temperatues are within Variance Range</t>
+  </si>
+  <si>
+    <t>Both portals show slightly similar Weather conditions!</t>
+  </si>
+  <si>
+    <t>Both portals show different Weather conditions!</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>3.3949999999999996</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>83</t>
+  </si>
+  <si>
+    <t>5.75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Humid and Partly Cloudy
 </t>
   </si>
   <si>
-    <t>64</t>
-  </si>
-  <si>
-    <t>7.15</t>
-  </si>
-  <si>
-    <t>29.00</t>
-  </si>
-  <si>
-    <t>89</t>
-  </si>
-  <si>
-    <t>Mist and mist</t>
-  </si>
-  <si>
-    <t>Rain and light rain</t>
-  </si>
-  <si>
-    <t>23.00</t>
-  </si>
-  <si>
-    <t>94</t>
-  </si>
-  <si>
-    <t>2.60</t>
-  </si>
-  <si>
-    <t>28.00</t>
-  </si>
-  <si>
-    <t>30.00</t>
-  </si>
-  <si>
-    <t>4.60</t>
-  </si>
-  <si>
-    <t>Haze and haze</t>
-  </si>
-  <si>
-    <t>1.78</t>
-  </si>
-  <si>
-    <t>26.00</t>
-  </si>
-  <si>
-    <t>3.10</t>
-  </si>
-  <si>
-    <t>28.97</t>
-  </si>
-  <si>
-    <t>68</t>
-  </si>
-  <si>
-    <t>5.47</t>
-  </si>
-  <si>
-    <t>Clouds and few clouds</t>
-  </si>
-  <si>
-    <t>4.97</t>
-  </si>
-  <si>
-    <t>Temperatues are NOT within Variance Range</t>
-  </si>
-  <si>
-    <t>Temperatues are within Variance Range</t>
+    <t>77</t>
+  </si>
+  <si>
+    <t>7.49</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>85</t>
+  </si>
+  <si>
+    <t>3.2199999999999998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overcast
+</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>5.53</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>7.41</t>
+  </si>
+  <si>
+    <t>1.50</t>
+  </si>
+  <si>
+    <t>28.57</t>
+  </si>
+  <si>
+    <t>73</t>
+  </si>
+  <si>
+    <t>5.10</t>
+  </si>
+  <si>
+    <t>30.07</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>7.04</t>
+  </si>
+  <si>
+    <t>Clouds and broken clouds</t>
+  </si>
+  <si>
+    <t>24.00</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>32.00</t>
+  </si>
+  <si>
+    <t>84</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -253,7 +253,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -264,6 +264,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -582,24 +583,24 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D2:D11"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="17.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="28.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="16.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="41.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="36.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="25.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="24.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="27.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="16.140625" collapsed="true"/>
-    <col min="10" max="10" style="1" width="9.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="24.42578125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="20.5703125" collapsed="true"/>
-    <col min="13" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="17.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="28.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="36.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="36.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="25" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="49.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="27.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="9.140625" style="1" collapsed="1"/>
+    <col min="11" max="11" width="24.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="20.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -647,192 +648,210 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" t="s">
-        <v>20</v>
+      <c r="G2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L2" t="s">
-        <v>21</v>
+        <v>48</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="L3" t="s">
-        <v>25</v>
+      <c r="L3" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="I4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="L4" t="s">
-        <v>29</v>
+      <c r="L4" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" t="s">
         <v>30</v>
       </c>
-      <c r="D5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="H5" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="L5" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I5" t="s">
-        <v>31</v>
-      </c>
-      <c r="K5" t="s">
-        <v>45</v>
-      </c>
-      <c r="L5" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" t="s">
+      <c r="B6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="L6" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="I6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K6" t="s">
-        <v>57</v>
-      </c>
-      <c r="L6" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="L7" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" t="s">
-        <v>40</v>
-      </c>
-      <c r="I7" t="s">
-        <v>37</v>
-      </c>
-      <c r="K7" t="s">
-        <v>48</v>
-      </c>
-      <c r="L7" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log4j implimentation and Commenting halfway done, code formatting halfway done
</commit_message>
<xml_diff>
--- a/src/main/resources/test/data/dataExcel.xlsx
+++ b/src/main/resources/test/data/dataExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cp\eclipse-workspace\WeatherReport0001\src\main\resources\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB068A1A-ED77-495C-B9CA-67493F7EF5A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C898C76-3360-4EC7-9DFF-7CD47C5476CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{BBC9B369-1E26-4ED4-AF77-86BE22BE0936}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="65">
   <si>
     <t>City</t>
   </si>
@@ -92,9 +92,6 @@
 </t>
   </si>
   <si>
-    <t>29</t>
-  </si>
-  <si>
     <t>29.00</t>
   </si>
   <si>
@@ -119,14 +116,6 @@
     <t>83</t>
   </si>
   <si>
-    <t xml:space="preserve">Humid and Partly Cloudy
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Overcast
-</t>
-  </si>
-  <si>
     <t>31</t>
   </si>
   <si>
@@ -178,39 +167,9 @@
     <t>65</t>
   </si>
   <si>
-    <t>70</t>
-  </si>
-  <si>
     <t>34</t>
   </si>
   <si>
-    <t>63</t>
-  </si>
-  <si>
-    <t>67</t>
-  </si>
-  <si>
-    <t>91</t>
-  </si>
-  <si>
-    <t>1.22</t>
-  </si>
-  <si>
-    <t>1.41</t>
-  </si>
-  <si>
-    <t>1.86</t>
-  </si>
-  <si>
-    <t>0.73</t>
-  </si>
-  <si>
-    <t>1.62</t>
-  </si>
-  <si>
-    <t>2.19</t>
-  </si>
-  <si>
     <t>Wind speed is faster on Open Weather Map.</t>
   </si>
   <si>
@@ -221,6 +180,48 @@
   </si>
   <si>
     <t>Temperatues are within Variance Range</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>1.23</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>1.60</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>1.61</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>0.94</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>1.66</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>2.42</t>
   </si>
 </sst>
 </file>
@@ -596,23 +597,23 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" customWidth="true" style="1" width="17.140625" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="28.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="16.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="16.5625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="41.28515625" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="36.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="25.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="25.02734375" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="49.42578125" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="27.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="16.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="16.14453125" collapsed="true"/>
     <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="45.7109375" collapsed="true"/>
     <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="24.42578125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="12.7109375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="12.73828125" collapsed="true"/>
     <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="40.85546875" collapsed="true"/>
     <col min="14" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
@@ -663,40 +664,40 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="M2" t="s">
         <v>47</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="J2" t="s">
-        <v>46</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="M2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -704,40 +705,40 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="I3" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="J3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>55</v>
       </c>
       <c r="M3" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -745,40 +746,40 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="J4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="M4" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -786,40 +787,40 @@
         <v>16</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J5" t="s">
         <v>42</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="J5" t="s">
-        <v>45</v>
-      </c>
       <c r="K5" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="M5" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -827,40 +828,40 @@
         <v>18</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="4" t="s">
+      <c r="I6" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J6" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="J6" t="s">
-        <v>45</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>33</v>
-      </c>
       <c r="L6" s="4" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="M6" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -868,40 +869,40 @@
         <v>17</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>63</v>
-      </c>
       <c r="E7" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="J7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="M7" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WebEvent Listner integration complete + reviewing code
</commit_message>
<xml_diff>
--- a/src/main/resources/test/data/dataExcel.xlsx
+++ b/src/main/resources/test/data/dataExcel.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="77">
   <si>
     <t>City</t>
   </si>
@@ -222,6 +222,42 @@
   </si>
   <si>
     <t>2.42</t>
+  </si>
+  <si>
+    <t>27.00</t>
+  </si>
+  <si>
+    <t>3.29</t>
+  </si>
+  <si>
+    <t>3.60</t>
+  </si>
+  <si>
+    <t>Clouds and scattered clouds</t>
+  </si>
+  <si>
+    <t>29.82</t>
+  </si>
+  <si>
+    <t>7.93</t>
+  </si>
+  <si>
+    <t>Clouds and overcast clouds</t>
+  </si>
+  <si>
+    <t>26.00</t>
+  </si>
+  <si>
+    <t>2.60</t>
+  </si>
+  <si>
+    <t>28.00</t>
+  </si>
+  <si>
+    <t>94</t>
+  </si>
+  <si>
+    <t>5.95</t>
   </si>
 </sst>
 </file>
@@ -603,16 +639,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" customWidth="true" style="1" width="17.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="28.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="28.28125" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="16.5625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="41.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="36.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="36.74609375" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="25.02734375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="49.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="27.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="49.4140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="27.86328125" collapsed="true"/>
     <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="16.14453125" collapsed="true"/>
     <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="45.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="24.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="24.45703125" collapsed="true"/>
     <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="12.73828125" collapsed="true"/>
     <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="40.85546875" collapsed="true"/>
     <col min="14" max="16384" style="1" width="9.140625" collapsed="true"/>
@@ -664,7 +700,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>51</v>
@@ -691,7 +727,7 @@
         <v>43</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>30</v>
+        <v>66</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>53</v>
@@ -705,16 +741,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>54</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>20</v>
@@ -723,7 +759,7 @@
         <v>27</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>45</v>
@@ -732,7 +768,7 @@
         <v>43</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>55</v>
@@ -746,16 +782,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>19</v>
@@ -764,7 +800,7 @@
         <v>26</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>56</v>
@@ -773,7 +809,7 @@
         <v>43</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>57</v>
@@ -787,7 +823,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>29</v>
@@ -796,16 +832,16 @@
         <v>49</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>58</v>
@@ -814,7 +850,7 @@
         <v>42</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>59</v>
@@ -855,7 +891,7 @@
         <v>42</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="L6" s="4" t="s">
         <v>62</v>
@@ -869,7 +905,7 @@
         <v>17</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>46</v>
@@ -887,7 +923,7 @@
         <v>26</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>63</v>
@@ -896,7 +932,7 @@
         <v>43</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="L7" s="4" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
Screenshot implemented, Webevent Listener implemented
</commit_message>
<xml_diff>
--- a/src/main/resources/test/data/dataExcel.xlsx
+++ b/src/main/resources/test/data/dataExcel.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="89">
   <si>
     <t>City</t>
   </si>
@@ -258,6 +258,42 @@
   </si>
   <si>
     <t>5.95</t>
+  </si>
+  <si>
+    <t>1.54</t>
+  </si>
+  <si>
+    <t>27.13</t>
+  </si>
+  <si>
+    <t>78</t>
+  </si>
+  <si>
+    <t>4.87</t>
+  </si>
+  <si>
+    <t>Rain and moderate rain</t>
+  </si>
+  <si>
+    <t>28.99</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>8.03</t>
+  </si>
+  <si>
+    <t>Clear and clear sky</t>
+  </si>
+  <si>
+    <t>25.00</t>
+  </si>
+  <si>
+    <t>4.60</t>
+  </si>
+  <si>
+    <t>2.10</t>
   </si>
 </sst>
 </file>
@@ -718,7 +754,7 @@
         <v>26</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>52</v>
@@ -727,7 +763,7 @@
         <v>43</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>53</v>
@@ -741,7 +777,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>54</v>
@@ -750,7 +786,7 @@
         <v>49</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>20</v>
@@ -759,7 +795,7 @@
         <v>27</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>28</v>
+        <v>79</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>45</v>
@@ -768,7 +804,7 @@
         <v>43</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>55</v>
@@ -782,7 +818,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>44</v>
@@ -791,7 +827,7 @@
         <v>50</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>19</v>
@@ -800,7 +836,7 @@
         <v>26</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>45</v>
+        <v>83</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>56</v>
@@ -809,7 +845,7 @@
         <v>43</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>57</v>
@@ -823,7 +859,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>29</v>
@@ -841,7 +877,7 @@
         <v>26</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>58</v>
@@ -850,7 +886,7 @@
         <v>42</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>59</v>
@@ -932,7 +968,7 @@
         <v>43</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="L7" s="4" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
Lots of cleanup, again!
</commit_message>
<xml_diff>
--- a/src/main/resources/test/data/dataExcel.xlsx
+++ b/src/main/resources/test/data/dataExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cp\eclipse-workspace\WeatherReport0001\src\main\resources\test\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parik\IdeaProjects\WeatehrReport001\src\main\resources\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7BA1FC1-E767-4418-AF66-8E8722F5CA28}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA92DAA-EA8E-46B0-A4D8-3CB910CE5D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{BBC9B369-1E26-4ED4-AF77-86BE22BE0936}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BBC9B369-1E26-4ED4-AF77-86BE22BE0936}"/>
   </bookViews>
   <sheets>
     <sheet name="listOfCities" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="48">
   <si>
     <t>City</t>
   </si>
@@ -76,55 +76,10 @@
     <t>Imphal</t>
   </si>
   <si>
-    <t>Blank Sheet.</t>
-  </si>
-  <si>
-    <t>Will open sheet again after test execution finishes.</t>
-  </si>
-  <si>
-    <t>28.00</t>
-  </si>
-  <si>
-    <t>88</t>
-  </si>
-  <si>
     <t>Mist and mist</t>
   </si>
   <si>
-    <t>27.00</t>
-  </si>
-  <si>
-    <t>83</t>
-  </si>
-  <si>
-    <t>28.99</t>
-  </si>
-  <si>
-    <t>72</t>
-  </si>
-  <si>
-    <t>Clouds and broken clouds</t>
-  </si>
-  <si>
-    <t>23.00</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>Thunderstorm and thunderstorm with heavy rain</t>
-  </si>
-  <si>
-    <t>34.07</t>
-  </si>
-  <si>
-    <t>54</t>
-  </si>
-  <si>
     <t>Clouds and scattered clouds</t>
-  </si>
-  <si>
-    <t>25.00</t>
   </si>
   <si>
     <t>94</t>
@@ -179,6 +134,45 @@
   </si>
   <si>
     <t>Both portals show different Weather conditions!</t>
+  </si>
+  <si>
+    <t>Clear and clear sky</t>
+  </si>
+  <si>
+    <t>89</t>
+  </si>
+  <si>
+    <t>Clouds and overcast clouds</t>
+  </si>
+  <si>
+    <t>26.99</t>
+  </si>
+  <si>
+    <t>25.04</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>25.74</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>27.96</t>
+  </si>
+  <si>
+    <t>29.98</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>19.15</t>
+  </si>
+  <si>
+    <t>97</t>
   </si>
 </sst>
 </file>
@@ -220,9 +214,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -241,9 +233,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -281,7 +273,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -387,7 +379,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -529,7 +521,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -540,20 +532,20 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="I4" sqref="I4:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" customWidth="true" style="1" width="17.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="28.28125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="16.5625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="28.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="16.5703125" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="41.20703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="44.9765625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="25.02734375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="36.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="25.0" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="49.4140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="27.86328125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="16.14453125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="27.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="16.140625" collapsed="true"/>
     <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="45.671875" collapsed="true"/>
     <col min="11" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
@@ -574,10 +566,10 @@
       <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -595,31 +587,31 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" t="s">
         <v>20</v>
       </c>
-      <c r="F2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" t="s">
-        <v>35</v>
-      </c>
       <c r="J2" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -627,31 +619,31 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
         <v>21</v>
       </c>
-      <c r="C3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>36</v>
-      </c>
       <c r="G3" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="H3" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="I3" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="J3" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -659,21 +651,27 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4"/>
-      <c r="D4"/>
+        <v>41</v>
+      </c>
+      <c r="C4" s="2">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F4"/>
       <c r="G4" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="H4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4"/>
+        <v>42</v>
+      </c>
+      <c r="I4" s="2">
+        <v>75</v>
+      </c>
       <c r="J4"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -681,21 +679,27 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5"/>
-      <c r="D5"/>
+        <v>43</v>
+      </c>
+      <c r="C5" s="2">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="F5"/>
       <c r="G5" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="H5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5"/>
+        <v>18</v>
+      </c>
+      <c r="I5" s="2">
+        <v>91</v>
+      </c>
       <c r="J5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -703,31 +707,31 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" t="s">
         <v>29</v>
-      </c>
-      <c r="C6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H6" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" t="s">
-        <v>40</v>
-      </c>
-      <c r="J6" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -735,31 +739,31 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
         <v>32</v>
       </c>
-      <c r="C7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" t="s">
-        <v>46</v>
-      </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="F7" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="G7" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="H7" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="I7" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="J7" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>